<commit_message>
Added a "Stop key" on Mono mode
</commit_message>
<xml_diff>
--- a/Fujiya Instruments/Junk Guitar/Junk Guitar/xlsx/VHG.xlsx
+++ b/Fujiya Instruments/Junk Guitar/Junk Guitar/xlsx/VHG.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADCEAFC-048B-4F4B-8F69-27E1D953B0EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2385" yWindow="3945" windowWidth="24825" windowHeight="15615" tabRatio="500"/>
+    <workbookView xWindow="1320" yWindow="1005" windowWidth="25365" windowHeight="14160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VHG Poly (Main)" sheetId="1" r:id="rId1"/>
@@ -26,12 +27,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>作成者</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -46,7 +47,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -66,12 +67,12 @@
 </file>
 
 <file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>作成者</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000001000000}">
       <text>
         <r>
           <rPr>
@@ -86,7 +87,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000002000000}">
       <text>
         <r>
           <rPr>
@@ -106,12 +107,12 @@
 </file>
 
 <file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>作成者</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -126,7 +127,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000002000000}">
       <text>
         <r>
           <rPr>
@@ -146,12 +147,12 @@
 </file>
 
 <file path=xl/comments12.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>作成者</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0B00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -166,7 +167,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0B00-000002000000}">
       <text>
         <r>
           <rPr>
@@ -186,12 +187,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>作成者</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -206,7 +207,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -226,12 +227,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>作成者</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -246,7 +247,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -266,12 +267,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>作成者</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -286,7 +287,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -306,12 +307,12 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>作成者</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -326,7 +327,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
       <text>
         <r>
           <rPr>
@@ -346,12 +347,12 @@
 </file>
 
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>作成者</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
       <text>
         <r>
           <rPr>
@@ -366,7 +367,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000002000000}">
       <text>
         <r>
           <rPr>
@@ -386,12 +387,12 @@
 </file>
 
 <file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>作成者</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
       <text>
         <r>
           <rPr>
@@ -406,7 +407,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000002000000}">
       <text>
         <r>
           <rPr>
@@ -426,12 +427,12 @@
 </file>
 
 <file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>作成者</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000001000000}">
       <text>
         <r>
           <rPr>
@@ -446,7 +447,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000002000000}">
       <text>
         <r>
           <rPr>
@@ -466,12 +467,12 @@
 </file>
 
 <file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>作成者</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000001000000}">
       <text>
         <r>
           <rPr>
@@ -486,7 +487,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000002000000}">
       <text>
         <r>
           <rPr>
@@ -506,7 +507,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="251">
   <si>
     <t>Name</t>
   </si>
@@ -1257,11 +1258,15 @@
   <si>
     <t>VHG Riff (Stop)</t>
   </si>
+  <si>
+    <t>Stop</t>
+    <phoneticPr fontId="7"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -1451,7 +1456,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1530,11 +1535,14 @@
     <xf numFmtId="49" fontId="3" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="説明文" xfId="1" builtinId="53" customBuiltin="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
-    <cellStyle name="標準 2" xfId="2"/>
+    <cellStyle name="標準 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1610,6 +1618,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1626,12 +1637,18 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1026" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="1026" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1925,15 +1942,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K131"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K132"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -1957,10 +1974,10 @@
       <c r="A1" s="25" t="s">
         <v>237</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="26" t="s">
         <v>238</v>
       </c>
-      <c r="C1" s="24"/>
+      <c r="C1" s="26"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="12" t="s">
@@ -2022,25 +2039,25 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
-        <v>143</v>
+        <v>250</v>
       </c>
       <c r="B5" s="19">
         <v>1</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D5" s="20" t="s">
+      <c r="C5" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D5" s="24" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="19">
         <v>1</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="G5" s="19">
-        <v>120</v>
+        <v>15</v>
       </c>
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
@@ -2049,13 +2066,13 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B6" s="19">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D6" s="20" t="s">
         <v>12</v>
@@ -2064,7 +2081,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G6" s="19">
         <v>120</v>
@@ -2076,13 +2093,13 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B7" s="19">
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D7" s="20" t="s">
         <v>12</v>
@@ -2091,7 +2108,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G7" s="19">
         <v>120</v>
@@ -2103,13 +2120,13 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B8" s="19">
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>12</v>
@@ -2118,7 +2135,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G8" s="19">
         <v>120</v>
@@ -2130,13 +2147,13 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B9" s="19">
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D9" s="20" t="s">
         <v>12</v>
@@ -2145,7 +2162,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G9" s="19">
         <v>120</v>
@@ -2157,13 +2174,13 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B10" s="19">
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>12</v>
@@ -2172,7 +2189,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G10" s="19">
         <v>120</v>
@@ -2184,13 +2201,13 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B11" s="19">
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>12</v>
@@ -2199,7 +2216,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G11" s="19">
         <v>120</v>
@@ -2211,13 +2228,13 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B12" s="19">
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D12" s="20" t="s">
         <v>12</v>
@@ -2226,7 +2243,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G12" s="19">
         <v>120</v>
@@ -2238,13 +2255,13 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B13" s="19">
         <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D13" s="20" t="s">
         <v>12</v>
@@ -2253,7 +2270,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G13" s="19">
         <v>120</v>
@@ -2265,13 +2282,13 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B14" s="19">
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D14" s="20" t="s">
         <v>12</v>
@@ -2280,7 +2297,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G14" s="19">
         <v>120</v>
@@ -2292,13 +2309,13 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B15" s="19">
         <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D15" s="20" t="s">
         <v>12</v>
@@ -2307,7 +2324,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G15" s="19">
         <v>120</v>
@@ -2319,13 +2336,13 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B16" s="19">
         <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D16" s="20" t="s">
         <v>12</v>
@@ -2334,7 +2351,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G16" s="19">
         <v>120</v>
@@ -2346,13 +2363,13 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B17" s="19">
         <v>1</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D17" s="20" t="s">
         <v>12</v>
@@ -2361,7 +2378,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G17" s="19">
         <v>120</v>
@@ -2373,13 +2390,13 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B18" s="19">
         <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D18" s="20" t="s">
         <v>12</v>
@@ -2388,7 +2405,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G18" s="19">
         <v>120</v>
@@ -2400,13 +2417,13 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B19" s="19">
         <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D19" s="20" t="s">
         <v>12</v>
@@ -2415,7 +2432,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G19" s="19">
         <v>120</v>
@@ -2427,13 +2444,13 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B20" s="19">
         <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D20" s="20" t="s">
         <v>12</v>
@@ -2442,7 +2459,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G20" s="19">
         <v>120</v>
@@ -2453,13 +2470,27 @@
       <c r="K20" s="19"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="1"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
+      <c r="A21" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B21" s="19">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="19">
+        <v>1</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="G21" s="19">
+        <v>120</v>
+      </c>
       <c r="H21" s="19"/>
       <c r="I21" s="19"/>
       <c r="J21" s="19"/>
@@ -3895,66 +3926,79 @@
       <c r="J131" s="19"/>
       <c r="K131" s="19"/>
     </row>
+    <row r="132" spans="1:11">
+      <c r="A132" s="1"/>
+      <c r="B132" s="19"/>
+      <c r="C132" s="2"/>
+      <c r="D132" s="20"/>
+      <c r="E132" s="19"/>
+      <c r="F132" s="19"/>
+      <c r="G132" s="19"/>
+      <c r="H132" s="19"/>
+      <c r="I132" s="19"/>
+      <c r="J132" s="19"/>
+      <c r="K132" s="19"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <phoneticPr fontId="7"/>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B132" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I132" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G132" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J132" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K132" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000005000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$B$2:$B$4</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D4:D131</xm:sqref>
+          <xm:sqref>D4:D132</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000006000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$C$2:$C$6</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>E4:E131</xm:sqref>
+          <xm:sqref>E4:E132</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty.">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty." xr:uid="{00000000-0002-0000-0000-000007000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$A$2:$A$258</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>F4:F131</xm:sqref>
+          <xm:sqref>F4:F132</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3963,7 +4007,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:K131"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3988,10 +4032,10 @@
       <c r="A1" s="25" t="s">
         <v>237</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="26" t="s">
         <v>247</v>
       </c>
-      <c r="C1" s="24"/>
+      <c r="C1" s="26"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="12" t="s">
@@ -5890,23 +5934,23 @@
   </mergeCells>
   <phoneticPr fontId="8"/>
   <dataValidations count="5">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131" xr:uid="{00000000-0002-0000-0900-000000000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131" xr:uid="{00000000-0002-0000-0900-000001000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131" xr:uid="{00000000-0002-0000-0900-000002000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131" xr:uid="{00000000-0002-0000-0900-000003000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131" xr:uid="{00000000-0002-0000-0900-000004000000}">
       <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5917,7 +5961,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty.">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty." xr:uid="{00000000-0002-0000-0900-000005000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$A$2:$A$258</xm:f>
           </x14:formula1>
@@ -5926,7 +5970,7 @@
           </x14:formula2>
           <xm:sqref>F4:F131</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0900-000006000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$C$2:$C$6</xm:f>
           </x14:formula1>
@@ -5935,7 +5979,7 @@
           </x14:formula2>
           <xm:sqref>E4:E131</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0900-000007000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$B$2:$B$4</xm:f>
           </x14:formula1>
@@ -5951,7 +5995,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:K131"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -5976,10 +6020,10 @@
       <c r="A1" s="25" t="s">
         <v>237</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="26" t="s">
         <v>248</v>
       </c>
-      <c r="C1" s="24"/>
+      <c r="C1" s="26"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="12" t="s">
@@ -7738,23 +7782,23 @@
   </mergeCells>
   <phoneticPr fontId="8"/>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131" xr:uid="{00000000-0002-0000-0A00-000000000000}">
       <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131" xr:uid="{00000000-0002-0000-0A00-000001000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131" xr:uid="{00000000-0002-0000-0A00-000002000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131" xr:uid="{00000000-0002-0000-0A00-000003000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131" xr:uid="{00000000-0002-0000-0A00-000004000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
@@ -7765,7 +7809,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0A00-000005000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$B$2:$B$4</xm:f>
           </x14:formula1>
@@ -7774,7 +7818,7 @@
           </x14:formula2>
           <xm:sqref>D4:D131</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0A00-000006000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$C$2:$C$6</xm:f>
           </x14:formula1>
@@ -7783,7 +7827,7 @@
           </x14:formula2>
           <xm:sqref>E4:E131</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty.">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty." xr:uid="{00000000-0002-0000-0A00-000007000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$A$2:$A$258</xm:f>
           </x14:formula1>
@@ -7799,7 +7843,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:K131"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -7824,10 +7868,10 @@
       <c r="A1" s="25" t="s">
         <v>237</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="26" t="s">
         <v>249</v>
       </c>
-      <c r="C1" s="24"/>
+      <c r="C1" s="26"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="12" t="s">
@@ -9768,23 +9812,23 @@
   </mergeCells>
   <phoneticPr fontId="8"/>
   <dataValidations count="5">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131" xr:uid="{00000000-0002-0000-0B00-000000000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131" xr:uid="{00000000-0002-0000-0B00-000001000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131" xr:uid="{00000000-0002-0000-0B00-000002000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131" xr:uid="{00000000-0002-0000-0B00-000003000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131" xr:uid="{00000000-0002-0000-0B00-000004000000}">
       <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -9795,7 +9839,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty.">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty." xr:uid="{00000000-0002-0000-0B00-000005000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$A$2:$A$258</xm:f>
           </x14:formula1>
@@ -9804,7 +9848,7 @@
           </x14:formula2>
           <xm:sqref>F4:F131</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0B00-000006000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$C$2:$C$6</xm:f>
           </x14:formula1>
@@ -9813,7 +9857,7 @@
           </x14:formula2>
           <xm:sqref>E4:E131</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0B00-000007000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$B$2:$B$4</xm:f>
           </x14:formula1>
@@ -9829,8 +9873,8 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <sheetPr>
     <tabColor rgb="FF000000"/>
   </sheetPr>
   <dimension ref="A1:C258"/>
@@ -11292,7 +11336,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K131"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -11317,10 +11361,10 @@
       <c r="A1" s="25" t="s">
         <v>237</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="26" t="s">
         <v>239</v>
       </c>
-      <c r="C1" s="24"/>
+      <c r="C1" s="26"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="12" t="s">
@@ -13109,23 +13153,23 @@
   </mergeCells>
   <phoneticPr fontId="8"/>
   <dataValidations count="5">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131" xr:uid="{00000000-0002-0000-0100-000004000000}">
       <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -13136,7 +13180,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty.">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty." xr:uid="{00000000-0002-0000-0100-000005000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$A$2:$A$258</xm:f>
           </x14:formula1>
@@ -13145,7 +13189,7 @@
           </x14:formula2>
           <xm:sqref>F4:F131</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000006000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$C$2:$C$6</xm:f>
           </x14:formula1>
@@ -13154,7 +13198,7 @@
           </x14:formula2>
           <xm:sqref>E4:E131</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000007000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$B$2:$B$4</xm:f>
           </x14:formula1>
@@ -13170,7 +13214,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K131"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -13195,10 +13239,10 @@
       <c r="A1" s="25" t="s">
         <v>237</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="26" t="s">
         <v>240</v>
       </c>
-      <c r="C1" s="24"/>
+      <c r="C1" s="26"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="12" t="s">
@@ -15195,23 +15239,23 @@
   </mergeCells>
   <phoneticPr fontId="8"/>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131" xr:uid="{00000000-0002-0000-0200-000003000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131" xr:uid="{00000000-0002-0000-0200-000004000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
@@ -15222,7 +15266,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000005000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$B$2:$B$4</xm:f>
           </x14:formula1>
@@ -15231,7 +15275,7 @@
           </x14:formula2>
           <xm:sqref>D4:D131</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000006000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$C$2:$C$6</xm:f>
           </x14:formula1>
@@ -15240,7 +15284,7 @@
           </x14:formula2>
           <xm:sqref>E4:E131</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty.">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty." xr:uid="{00000000-0002-0000-0200-000007000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$A$2:$A$258</xm:f>
           </x14:formula1>
@@ -15256,7 +15300,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K131"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -15281,10 +15325,10 @@
       <c r="A1" s="25" t="s">
         <v>237</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="26" t="s">
         <v>241</v>
       </c>
-      <c r="C1" s="24"/>
+      <c r="C1" s="26"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="12" t="s">
@@ -17043,23 +17087,23 @@
   </mergeCells>
   <phoneticPr fontId="8"/>
   <dataValidations count="5">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131" xr:uid="{00000000-0002-0000-0300-000002000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131" xr:uid="{00000000-0002-0000-0300-000003000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131" xr:uid="{00000000-0002-0000-0300-000004000000}">
       <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -17070,7 +17114,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty.">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty." xr:uid="{00000000-0002-0000-0300-000005000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$A$2:$A$258</xm:f>
           </x14:formula1>
@@ -17079,7 +17123,7 @@
           </x14:formula2>
           <xm:sqref>F4:F131</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000006000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$C$2:$C$6</xm:f>
           </x14:formula1>
@@ -17088,7 +17132,7 @@
           </x14:formula2>
           <xm:sqref>E4:E131</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000007000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$B$2:$B$4</xm:f>
           </x14:formula1>
@@ -17104,7 +17148,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K131"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -17129,10 +17173,10 @@
       <c r="A1" s="25" t="s">
         <v>237</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="26" t="s">
         <v>242</v>
       </c>
-      <c r="C1" s="24"/>
+      <c r="C1" s="26"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="12" t="s">
@@ -19073,23 +19117,23 @@
   </mergeCells>
   <phoneticPr fontId="8"/>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131" xr:uid="{00000000-0002-0000-0400-000001000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131" xr:uid="{00000000-0002-0000-0400-000002000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131" xr:uid="{00000000-0002-0000-0400-000003000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131" xr:uid="{00000000-0002-0000-0400-000004000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
@@ -19100,7 +19144,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000005000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$B$2:$B$4</xm:f>
           </x14:formula1>
@@ -19109,7 +19153,7 @@
           </x14:formula2>
           <xm:sqref>D4:D131</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000006000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$C$2:$C$6</xm:f>
           </x14:formula1>
@@ -19118,7 +19162,7 @@
           </x14:formula2>
           <xm:sqref>E4:E131</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty.">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty." xr:uid="{00000000-0002-0000-0400-000007000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$A$2:$A$258</xm:f>
           </x14:formula1>
@@ -19134,7 +19178,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K131"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -19159,10 +19203,10 @@
       <c r="A1" s="25" t="s">
         <v>237</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="C1" s="24"/>
+      <c r="C1" s="26"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="12" t="s">
@@ -21215,23 +21259,23 @@
   </mergeCells>
   <phoneticPr fontId="8"/>
   <dataValidations count="5">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131" xr:uid="{00000000-0002-0000-0500-000001000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131" xr:uid="{00000000-0002-0000-0500-000002000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131" xr:uid="{00000000-0002-0000-0500-000003000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131" xr:uid="{00000000-0002-0000-0500-000004000000}">
       <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -21242,7 +21286,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty.">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty." xr:uid="{00000000-0002-0000-0500-000005000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$A$2:$A$258</xm:f>
           </x14:formula1>
@@ -21251,7 +21295,7 @@
           </x14:formula2>
           <xm:sqref>F4:F131</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000006000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$C$2:$C$6</xm:f>
           </x14:formula1>
@@ -21260,7 +21304,7 @@
           </x14:formula2>
           <xm:sqref>E4:E131</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000007000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$B$2:$B$4</xm:f>
           </x14:formula1>
@@ -21276,7 +21320,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K131"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -21301,10 +21345,10 @@
       <c r="A1" s="25" t="s">
         <v>237</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="26" t="s">
         <v>244</v>
       </c>
-      <c r="C1" s="24"/>
+      <c r="C1" s="26"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="12" t="s">
@@ -23077,23 +23121,23 @@
   </mergeCells>
   <phoneticPr fontId="8"/>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131" xr:uid="{00000000-0002-0000-0600-000000000000}">
       <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131" xr:uid="{00000000-0002-0000-0600-000001000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131" xr:uid="{00000000-0002-0000-0600-000002000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131" xr:uid="{00000000-0002-0000-0600-000003000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131" xr:uid="{00000000-0002-0000-0600-000004000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
@@ -23104,7 +23148,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000005000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$B$2:$B$4</xm:f>
           </x14:formula1>
@@ -23113,7 +23157,7 @@
           </x14:formula2>
           <xm:sqref>D4:D131</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000006000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$C$2:$C$6</xm:f>
           </x14:formula1>
@@ -23122,7 +23166,7 @@
           </x14:formula2>
           <xm:sqref>E4:E131</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty.">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty." xr:uid="{00000000-0002-0000-0600-000007000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$A$2:$A$258</xm:f>
           </x14:formula1>
@@ -23138,7 +23182,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K131"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -23163,10 +23207,10 @@
       <c r="A1" s="25" t="s">
         <v>237</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="26" t="s">
         <v>245</v>
       </c>
-      <c r="C1" s="24"/>
+      <c r="C1" s="26"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="12" t="s">
@@ -24911,23 +24955,23 @@
   </mergeCells>
   <phoneticPr fontId="8"/>
   <dataValidations count="5">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131" xr:uid="{00000000-0002-0000-0700-000000000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131" xr:uid="{00000000-0002-0000-0700-000001000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131" xr:uid="{00000000-0002-0000-0700-000002000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131" xr:uid="{00000000-0002-0000-0700-000003000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131" xr:uid="{00000000-0002-0000-0700-000004000000}">
       <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -24938,7 +24982,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty.">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty." xr:uid="{00000000-0002-0000-0700-000005000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$A$2:$A$258</xm:f>
           </x14:formula1>
@@ -24947,7 +24991,7 @@
           </x14:formula2>
           <xm:sqref>F4:F131</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000006000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$C$2:$C$6</xm:f>
           </x14:formula1>
@@ -24956,7 +25000,7 @@
           </x14:formula2>
           <xm:sqref>E4:E131</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000007000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$B$2:$B$4</xm:f>
           </x14:formula1>
@@ -24972,7 +25016,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:K131"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -24997,10 +25041,10 @@
       <c r="A1" s="25" t="s">
         <v>237</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="26" t="s">
         <v>246</v>
       </c>
-      <c r="C1" s="24"/>
+      <c r="C1" s="26"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="12" t="s">
@@ -26829,23 +26873,23 @@
   </mergeCells>
   <phoneticPr fontId="8"/>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131" xr:uid="{00000000-0002-0000-0800-000002000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131" xr:uid="{00000000-0002-0000-0800-000003000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131" xr:uid="{00000000-0002-0000-0800-000004000000}">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
@@ -26856,7 +26900,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0800-000005000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$B$2:$B$4</xm:f>
           </x14:formula1>
@@ -26865,7 +26909,7 @@
           </x14:formula2>
           <xm:sqref>D4:D131</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0800-000006000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$C$2:$C$6</xm:f>
           </x14:formula1>
@@ -26874,7 +26918,7 @@
           </x14:formula2>
           <xm:sqref>E4:E131</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty.">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty." xr:uid="{00000000-0002-0000-0800-000007000000}">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$A$2:$A$258</xm:f>
           </x14:formula1>

</xml_diff>